<commit_message>
Drew attention to Excel validation errors.
git-svn-id: https://subversion.assembla.com/svn/treesdb/branches/ExcelImport@307 d913c9e1-59cf-094f-9d4b-ab1779aea92f
</commit_message>
<xml_diff>
--- a/TMD.UnitTests/Model/Import/Portable_TMD.xlsx
+++ b/TMD.UnitTests/Model/Import/Portable_TMD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-795" yWindow="6810" windowWidth="18840" windowHeight="7995" tabRatio="408" activeTab="3"/>
+    <workbookView xWindow="-795" yWindow="6810" windowWidth="18840" windowHeight="7995" tabRatio="408"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="3665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4204" uniqueCount="3664">
   <si>
     <t>Latitude</t>
   </si>
@@ -11144,9 +11144,6 @@
     <t>Publicize Coordinates</t>
   </si>
   <si>
-    <t>Styles</t>
-  </si>
-  <si>
     <t>hello world</t>
   </si>
 </sst>
@@ -11154,7 +11151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11261,15 +11258,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11304,11 +11294,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -11450,7 +11435,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11481,9 +11466,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -11511,7 +11495,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="30"/>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -11544,11 +11527,10 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="30">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
-    <cellStyle name="Bad" xfId="30" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -12030,7 +12012,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12726,92 +12708,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>3589</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>3591</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>3588</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>3546</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>3547</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>3537</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="20" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="19" t="s">
         <v>3536</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="20" t="s">
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="19" t="s">
         <v>3535</v>
       </c>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="20" t="s">
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="19" t="s">
         <v>3532</v>
       </c>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="20" t="s">
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="19" t="s">
         <v>3534</v>
       </c>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="20" t="s">
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="19" t="s">
         <v>3533</v>
       </c>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="20" t="s">
+      <c r="AP1" s="20"/>
+      <c r="AQ1" s="20"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="19" t="s">
         <v>3538</v>
       </c>
-      <c r="AT1" s="21"/>
-      <c r="AU1" s="21"/>
-      <c r="AV1" s="21"/>
-      <c r="AW1" s="21"/>
-      <c r="AX1" s="21"/>
-      <c r="AY1" s="21"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="19" t="s">
+      <c r="AT1" s="20"/>
+      <c r="AU1" s="20"/>
+      <c r="AV1" s="20"/>
+      <c r="AW1" s="20"/>
+      <c r="AX1" s="20"/>
+      <c r="AY1" s="20"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="18" t="s">
         <v>3661</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="16" t="s">
         <v>120</v>
       </c>
@@ -12929,7 +12911,7 @@
       <c r="AR2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AS2" s="18" t="s">
+      <c r="AS2" s="17" t="s">
         <v>3638</v>
       </c>
       <c r="AT2" s="4" t="s">
@@ -12953,7 +12935,7 @@
       <c r="AZ2" s="4" t="s">
         <v>3542</v>
       </c>
-      <c r="BA2" s="19"/>
+      <c r="BA2" s="18"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -13709,7 +13691,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -13791,7 +13773,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
     </row>
   </sheetData>
@@ -13822,11 +13804,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:R1825"/>
+  <dimension ref="A1:Q1825"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13850,7 +13832,7 @@
     <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -13902,11 +13884,8 @@
       <c r="Q1" s="1" t="s">
         <v>3579</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>3663</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -13958,9 +13937,8 @@
       <c r="Q2" s="1" t="s">
         <v>3584</v>
       </c>
-      <c r="R2" s="17"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -14013,7 +13991,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -14054,7 +14032,7 @@
         <v>3586</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -14089,7 +14067,7 @@
         <v>3581</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>77</v>
       </c>
@@ -14118,7 +14096,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -14144,7 +14122,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -14164,7 +14142,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -14181,7 +14159,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -14195,7 +14173,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>76</v>
       </c>
@@ -14209,7 +14187,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -14223,7 +14201,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -14237,7 +14215,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -14251,7 +14229,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
@@ -14265,7 +14243,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>75</v>
       </c>

</xml_diff>